<commit_message>
Nykaa test case 7 is working fine
</commit_message>
<xml_diff>
--- a/Project/testdata/GetAppData.xlsx
+++ b/Project/testdata/GetAppData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -412,9 +412,14 @@
         <v>Kajal</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>600001</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes on assert and author name
</commit_message>
<xml_diff>
--- a/Project/testdata/GetAppData.xlsx
+++ b/Project/testdata/GetAppData.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,20 +406,64 @@
       <c r="A1" t="str">
         <v>9123456789</v>
       </c>
+      <c r="B1" t="str">
+        <v>CATEGORIES</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>Kajal</v>
       </c>
+      <c r="B2" t="str">
+        <v>Customers also Viewed</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>600001</v>
       </c>
+      <c r="B3" t="str">
+        <v>BEAUTY TO GO</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="str">
+        <v>Terms &amp; Conditions</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="str">
+        <v>How does the delivery process work?</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="str">
+        <v>Privacy Policy</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="str">
+        <v>Whey Protein</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="str">
+        <v>Chennai</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="str">
+        <v>Sign in</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>